<commit_message>
Version 2 of Diplom
</commit_message>
<xml_diff>
--- a/full_file.xlsx
+++ b/full_file.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616"/>
   </bookViews>
   <sheets>
     <sheet name="teams" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
   <si>
     <t>group</t>
   </si>
@@ -56,31 +56,10 @@
     <t>Маркин Михаил Юрьевич</t>
   </si>
   <si>
-    <t>Соломеин Александр Сергеевич</t>
-  </si>
-  <si>
-    <t>РИМ-220906</t>
-  </si>
-  <si>
-    <t>Зенком Мирослав Владимирович</t>
-  </si>
-  <si>
-    <t>ЭН-470004</t>
-  </si>
-  <si>
-    <t>Иванов И</t>
-  </si>
-  <si>
-    <t>Петров Петр</t>
-  </si>
-  <si>
-    <t>РИ-111222</t>
-  </si>
-  <si>
-    <t>Сергеев Сергей Сергеевич</t>
-  </si>
-  <si>
-    <t>Сидоров Я</t>
+    <t>РИМ-220909</t>
+  </si>
+  <si>
+    <t>Иванов Иван Иванович</t>
   </si>
   <si>
     <t>index</t>
@@ -466,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -513,68 +492,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5">
         <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -587,36 +511,37 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="62.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="62.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -629,7 +554,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -640,10 +565,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -651,7 +576,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -671,10 +596,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -682,7 +607,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -692,20 +617,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -713,7 +638,15 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -725,18 +658,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -744,7 +677,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>